<commit_message>
backlog : suppression WS + API Post Parcours
</commit_message>
<xml_diff>
--- a/doc/2014/AconitBacklogV2.xlsx
+++ b/doc/2014/AconitBacklogV2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr filterPrivacy="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="28760" yWindow="1720" windowWidth="25600" windowHeight="16060" tabRatio="824" activeTab="5"/>
+    <workbookView xWindow="29180" yWindow="-440" windowWidth="25600" windowHeight="20480" tabRatio="824" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Accueil" sheetId="1" r:id="rId1"/>
@@ -1994,10 +1994,6 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" indent="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" indent="1"/>
       <protection locked="0"/>
@@ -2034,6 +2030,10 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" indent="1"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3013,11 +3013,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="353748664"/>
-        <c:axId val="353732664"/>
+        <c:axId val="420193400"/>
+        <c:axId val="420196584"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="353748664"/>
+        <c:axId val="420193400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3044,7 +3044,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="353732664"/>
+        <c:crossAx val="420196584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3052,7 +3052,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="353732664"/>
+        <c:axId val="420196584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3085,7 +3085,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="353748664"/>
+        <c:crossAx val="420193400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3502,11 +3502,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="317432248"/>
-        <c:axId val="317435432"/>
+        <c:axId val="420412024"/>
+        <c:axId val="420415208"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="317432248"/>
+        <c:axId val="420412024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3533,7 +3533,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="317435432"/>
+        <c:crossAx val="420415208"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3541,7 +3541,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="317435432"/>
+        <c:axId val="420415208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3574,7 +3574,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="317432248"/>
+        <c:crossAx val="420412024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3758,61 +3758,61 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>81.0</c:v>
+                  <c:v>80.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>76.73684210526315</c:v>
+                  <c:v>75.7894736842105</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>72.4736842105263</c:v>
+                  <c:v>71.57894736842104</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>68.21052631578945</c:v>
+                  <c:v>67.36842105263156</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>63.94736842105261</c:v>
+                  <c:v>63.15789473684209</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>59.68421052631577</c:v>
+                  <c:v>58.94736842105262</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>55.42105263157892</c:v>
+                  <c:v>54.73684210526314</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>51.15789473684208</c:v>
+                  <c:v>50.52631578947367</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>46.89473684210523</c:v>
+                  <c:v>46.3157894736842</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>42.6315789473684</c:v>
+                  <c:v>42.10526315789473</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>38.36842105263155</c:v>
+                  <c:v>37.89473684210525</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>34.10526315789471</c:v>
+                  <c:v>33.68421052631578</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>29.84210526315787</c:v>
+                  <c:v>29.47368421052631</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>25.57894736842103</c:v>
+                  <c:v>25.26315789473684</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>21.31578947368418</c:v>
+                  <c:v>21.05263157894736</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>17.05263157894734</c:v>
+                  <c:v>16.84210526315789</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>12.7894736842105</c:v>
+                  <c:v>12.63157894736842</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>8.526315789473657</c:v>
+                  <c:v>8.421052631578945</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>4.263157894736814</c:v>
+                  <c:v>4.210526315789472</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3972,11 +3972,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="317501224"/>
-        <c:axId val="317504376"/>
+        <c:axId val="431071144"/>
+        <c:axId val="431074296"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="317501224"/>
+        <c:axId val="431071144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4003,14 +4003,14 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="317504376"/>
+        <c:crossAx val="431074296"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="317504376"/>
+        <c:axId val="431074296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4043,7 +4043,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="317501224"/>
+        <c:crossAx val="431071144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4136,7 +4136,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -4523,11 +4522,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="354084904"/>
-        <c:axId val="354088088"/>
+        <c:axId val="431221944"/>
+        <c:axId val="431225128"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="354084904"/>
+        <c:axId val="431221944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4554,7 +4553,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="354088088"/>
+        <c:crossAx val="431225128"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4562,7 +4561,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="354088088"/>
+        <c:axId val="431225128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4595,14 +4594,13 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="354084904"/>
+        <c:crossAx val="431221944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -4688,7 +4686,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -5075,11 +5072,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="317673448"/>
-        <c:axId val="317676632"/>
+        <c:axId val="431353768"/>
+        <c:axId val="431356952"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="317673448"/>
+        <c:axId val="431353768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5106,7 +5103,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="317676632"/>
+        <c:crossAx val="431356952"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5114,7 +5111,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="317676632"/>
+        <c:axId val="431356952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5147,14 +5144,13 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="317673448"/>
+        <c:crossAx val="431353768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -5782,17 +5778,17 @@
       <c r="B3" s="5"/>
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
-      <c r="E3" s="167" t="s">
+      <c r="E3" s="166" t="s">
         <v>245</v>
       </c>
-      <c r="F3" s="167"/>
-      <c r="G3" s="167"/>
-      <c r="H3" s="167"/>
-      <c r="I3" s="167"/>
-      <c r="J3" s="167"/>
-      <c r="K3" s="167"/>
-      <c r="L3" s="167"/>
-      <c r="M3" s="167"/>
+      <c r="F3" s="166"/>
+      <c r="G3" s="166"/>
+      <c r="H3" s="166"/>
+      <c r="I3" s="166"/>
+      <c r="J3" s="166"/>
+      <c r="K3" s="166"/>
+      <c r="L3" s="166"/>
+      <c r="M3" s="166"/>
       <c r="N3" s="6"/>
       <c r="O3" s="6"/>
       <c r="P3" s="7"/>
@@ -5801,15 +5797,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
-      <c r="E4" s="167"/>
-      <c r="F4" s="167"/>
-      <c r="G4" s="167"/>
-      <c r="H4" s="167"/>
-      <c r="I4" s="167"/>
-      <c r="J4" s="167"/>
-      <c r="K4" s="167"/>
-      <c r="L4" s="167"/>
-      <c r="M4" s="167"/>
+      <c r="E4" s="166"/>
+      <c r="F4" s="166"/>
+      <c r="G4" s="166"/>
+      <c r="H4" s="166"/>
+      <c r="I4" s="166"/>
+      <c r="J4" s="166"/>
+      <c r="K4" s="166"/>
+      <c r="L4" s="166"/>
+      <c r="M4" s="166"/>
       <c r="N4" s="6"/>
       <c r="O4" s="6"/>
       <c r="P4" s="7"/>
@@ -5818,15 +5814,15 @@
       <c r="B5" s="5"/>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
-      <c r="E5" s="167"/>
-      <c r="F5" s="167"/>
-      <c r="G5" s="167"/>
-      <c r="H5" s="167"/>
-      <c r="I5" s="167"/>
-      <c r="J5" s="167"/>
-      <c r="K5" s="167"/>
-      <c r="L5" s="167"/>
-      <c r="M5" s="167"/>
+      <c r="E5" s="166"/>
+      <c r="F5" s="166"/>
+      <c r="G5" s="166"/>
+      <c r="H5" s="166"/>
+      <c r="I5" s="166"/>
+      <c r="J5" s="166"/>
+      <c r="K5" s="166"/>
+      <c r="L5" s="166"/>
+      <c r="M5" s="166"/>
       <c r="N5" s="6"/>
       <c r="O5" s="6"/>
       <c r="P5" s="7"/>
@@ -5901,55 +5897,55 @@
     </row>
     <row r="10" spans="2:16" ht="15" customHeight="1">
       <c r="B10" s="5"/>
-      <c r="C10" s="168" t="s">
+      <c r="C10" s="167" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="169"/>
-      <c r="E10" s="169"/>
-      <c r="F10" s="169"/>
-      <c r="G10" s="169"/>
-      <c r="H10" s="169"/>
-      <c r="I10" s="169"/>
-      <c r="J10" s="169"/>
-      <c r="K10" s="169"/>
-      <c r="L10" s="169"/>
-      <c r="M10" s="169"/>
-      <c r="N10" s="169"/>
-      <c r="O10" s="170"/>
+      <c r="D10" s="168"/>
+      <c r="E10" s="168"/>
+      <c r="F10" s="168"/>
+      <c r="G10" s="168"/>
+      <c r="H10" s="168"/>
+      <c r="I10" s="168"/>
+      <c r="J10" s="168"/>
+      <c r="K10" s="168"/>
+      <c r="L10" s="168"/>
+      <c r="M10" s="168"/>
+      <c r="N10" s="168"/>
+      <c r="O10" s="169"/>
       <c r="P10" s="7"/>
     </row>
     <row r="11" spans="2:16" ht="15" customHeight="1">
       <c r="B11" s="5"/>
-      <c r="C11" s="171"/>
-      <c r="D11" s="172"/>
-      <c r="E11" s="172"/>
-      <c r="F11" s="172"/>
-      <c r="G11" s="172"/>
-      <c r="H11" s="172"/>
-      <c r="I11" s="172"/>
-      <c r="J11" s="172"/>
-      <c r="K11" s="172"/>
-      <c r="L11" s="172"/>
-      <c r="M11" s="172"/>
-      <c r="N11" s="172"/>
-      <c r="O11" s="173"/>
+      <c r="C11" s="170"/>
+      <c r="D11" s="171"/>
+      <c r="E11" s="171"/>
+      <c r="F11" s="171"/>
+      <c r="G11" s="171"/>
+      <c r="H11" s="171"/>
+      <c r="I11" s="171"/>
+      <c r="J11" s="171"/>
+      <c r="K11" s="171"/>
+      <c r="L11" s="171"/>
+      <c r="M11" s="171"/>
+      <c r="N11" s="171"/>
+      <c r="O11" s="172"/>
       <c r="P11" s="7"/>
     </row>
     <row r="12" spans="2:16" ht="15" customHeight="1">
       <c r="B12" s="5"/>
-      <c r="C12" s="174"/>
-      <c r="D12" s="175"/>
-      <c r="E12" s="175"/>
-      <c r="F12" s="175"/>
-      <c r="G12" s="175"/>
-      <c r="H12" s="175"/>
-      <c r="I12" s="175"/>
-      <c r="J12" s="175"/>
-      <c r="K12" s="175"/>
-      <c r="L12" s="175"/>
-      <c r="M12" s="175"/>
-      <c r="N12" s="175"/>
-      <c r="O12" s="176"/>
+      <c r="C12" s="173"/>
+      <c r="D12" s="174"/>
+      <c r="E12" s="174"/>
+      <c r="F12" s="174"/>
+      <c r="G12" s="174"/>
+      <c r="H12" s="174"/>
+      <c r="I12" s="174"/>
+      <c r="J12" s="174"/>
+      <c r="K12" s="174"/>
+      <c r="L12" s="174"/>
+      <c r="M12" s="174"/>
+      <c r="N12" s="174"/>
+      <c r="O12" s="175"/>
       <c r="P12" s="7"/>
     </row>
     <row r="13" spans="2:16">
@@ -5971,27 +5967,27 @@
     </row>
     <row r="14" spans="2:16">
       <c r="B14" s="5"/>
-      <c r="C14" s="177" t="s">
-        <v>1</v>
-      </c>
-      <c r="D14" s="177"/>
-      <c r="E14" s="177" t="s">
-        <v>0</v>
-      </c>
-      <c r="F14" s="177"/>
-      <c r="G14" s="177"/>
-      <c r="H14" s="177" t="s">
+      <c r="C14" s="176" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="176"/>
+      <c r="E14" s="176" t="s">
+        <v>0</v>
+      </c>
+      <c r="F14" s="176"/>
+      <c r="G14" s="176"/>
+      <c r="H14" s="176" t="s">
         <v>2</v>
       </c>
-      <c r="I14" s="177"/>
-      <c r="J14" s="177" t="s">
+      <c r="I14" s="176"/>
+      <c r="J14" s="176" t="s">
         <v>53</v>
       </c>
-      <c r="K14" s="177"/>
-      <c r="L14" s="177"/>
-      <c r="M14" s="177"/>
-      <c r="N14" s="177"/>
-      <c r="O14" s="177"/>
+      <c r="K14" s="176"/>
+      <c r="L14" s="176"/>
+      <c r="M14" s="176"/>
+      <c r="N14" s="176"/>
+      <c r="O14" s="176"/>
       <c r="P14" s="7"/>
     </row>
     <row r="15" spans="2:16">
@@ -6009,14 +6005,14 @@
         <v>3</v>
       </c>
       <c r="I15" s="162"/>
-      <c r="J15" s="166" t="s">
+      <c r="J15" s="165" t="s">
         <v>33</v>
       </c>
-      <c r="K15" s="166"/>
-      <c r="L15" s="166"/>
-      <c r="M15" s="166"/>
-      <c r="N15" s="166"/>
-      <c r="O15" s="166"/>
+      <c r="K15" s="165"/>
+      <c r="L15" s="165"/>
+      <c r="M15" s="165"/>
+      <c r="N15" s="165"/>
+      <c r="O15" s="165"/>
       <c r="P15" s="7"/>
     </row>
     <row r="16" spans="2:16">
@@ -6034,14 +6030,14 @@
         <v>247</v>
       </c>
       <c r="I16" s="162"/>
-      <c r="J16" s="166" t="s">
+      <c r="J16" s="165" t="s">
         <v>248</v>
       </c>
-      <c r="K16" s="166"/>
-      <c r="L16" s="166"/>
-      <c r="M16" s="166"/>
-      <c r="N16" s="166"/>
-      <c r="O16" s="166"/>
+      <c r="K16" s="165"/>
+      <c r="L16" s="165"/>
+      <c r="M16" s="165"/>
+      <c r="N16" s="165"/>
+      <c r="O16" s="165"/>
       <c r="P16" s="7"/>
     </row>
     <row r="17" spans="2:16">
@@ -6053,12 +6049,12 @@
       <c r="G17" s="162"/>
       <c r="H17" s="162"/>
       <c r="I17" s="162"/>
-      <c r="J17" s="166"/>
-      <c r="K17" s="166"/>
-      <c r="L17" s="166"/>
-      <c r="M17" s="166"/>
-      <c r="N17" s="166"/>
-      <c r="O17" s="166"/>
+      <c r="J17" s="165"/>
+      <c r="K17" s="165"/>
+      <c r="L17" s="165"/>
+      <c r="M17" s="165"/>
+      <c r="N17" s="165"/>
+      <c r="O17" s="165"/>
       <c r="P17" s="7"/>
     </row>
     <row r="18" spans="2:16">
@@ -6070,12 +6066,12 @@
       <c r="G18" s="162"/>
       <c r="H18" s="162"/>
       <c r="I18" s="162"/>
-      <c r="J18" s="166"/>
-      <c r="K18" s="166"/>
-      <c r="L18" s="166"/>
-      <c r="M18" s="166"/>
-      <c r="N18" s="166"/>
-      <c r="O18" s="166"/>
+      <c r="J18" s="165"/>
+      <c r="K18" s="165"/>
+      <c r="L18" s="165"/>
+      <c r="M18" s="165"/>
+      <c r="N18" s="165"/>
+      <c r="O18" s="165"/>
       <c r="P18" s="7"/>
     </row>
     <row r="19" spans="2:16">
@@ -6087,12 +6083,12 @@
       <c r="G19" s="162"/>
       <c r="H19" s="162"/>
       <c r="I19" s="162"/>
-      <c r="J19" s="166"/>
-      <c r="K19" s="166"/>
-      <c r="L19" s="166"/>
-      <c r="M19" s="166"/>
-      <c r="N19" s="166"/>
-      <c r="O19" s="166"/>
+      <c r="J19" s="165"/>
+      <c r="K19" s="165"/>
+      <c r="L19" s="165"/>
+      <c r="M19" s="165"/>
+      <c r="N19" s="165"/>
+      <c r="O19" s="165"/>
       <c r="P19" s="7"/>
     </row>
     <row r="20" spans="2:16">
@@ -6104,12 +6100,12 @@
       <c r="G20" s="162"/>
       <c r="H20" s="162"/>
       <c r="I20" s="162"/>
-      <c r="J20" s="166"/>
-      <c r="K20" s="166"/>
-      <c r="L20" s="166"/>
-      <c r="M20" s="166"/>
-      <c r="N20" s="166"/>
-      <c r="O20" s="166"/>
+      <c r="J20" s="165"/>
+      <c r="K20" s="165"/>
+      <c r="L20" s="165"/>
+      <c r="M20" s="165"/>
+      <c r="N20" s="165"/>
+      <c r="O20" s="165"/>
       <c r="P20" s="7"/>
     </row>
     <row r="21" spans="2:16">
@@ -6121,12 +6117,12 @@
       <c r="G21" s="162"/>
       <c r="H21" s="162"/>
       <c r="I21" s="162"/>
-      <c r="J21" s="165"/>
-      <c r="K21" s="165"/>
-      <c r="L21" s="165"/>
-      <c r="M21" s="165"/>
-      <c r="N21" s="165"/>
-      <c r="O21" s="165"/>
+      <c r="J21" s="177"/>
+      <c r="K21" s="177"/>
+      <c r="L21" s="177"/>
+      <c r="M21" s="177"/>
+      <c r="N21" s="177"/>
+      <c r="O21" s="177"/>
       <c r="P21" s="7"/>
     </row>
     <row r="22" spans="2:16">
@@ -6138,12 +6134,12 @@
       <c r="G22" s="162"/>
       <c r="H22" s="162"/>
       <c r="I22" s="162"/>
-      <c r="J22" s="165"/>
-      <c r="K22" s="165"/>
-      <c r="L22" s="165"/>
-      <c r="M22" s="165"/>
-      <c r="N22" s="165"/>
-      <c r="O22" s="165"/>
+      <c r="J22" s="177"/>
+      <c r="K22" s="177"/>
+      <c r="L22" s="177"/>
+      <c r="M22" s="177"/>
+      <c r="N22" s="177"/>
+      <c r="O22" s="177"/>
       <c r="P22" s="7"/>
     </row>
     <row r="23" spans="2:16">
@@ -6337,68 +6333,6 @@
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
   <mergeCells count="78">
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="E32:G32"/>
-    <mergeCell ref="H32:I32"/>
-    <mergeCell ref="J32:O32"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="E30:G30"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="J30:O30"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="E31:G31"/>
-    <mergeCell ref="H31:I31"/>
-    <mergeCell ref="J31:O31"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="J28:O28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="E29:G29"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="J29:O29"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="E25:G25"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="J25:O25"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="E27:G27"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="J27:O27"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="J26:O26"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="J24:O24"/>
-    <mergeCell ref="E17:G17"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="J17:O17"/>
-    <mergeCell ref="E18:G18"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="J18:O18"/>
-    <mergeCell ref="E19:G19"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="E3:M5"/>
-    <mergeCell ref="C10:O12"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="J14:O14"/>
-    <mergeCell ref="E15:G15"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="J15:O15"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="J16:O16"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="J19:O19"/>
     <mergeCell ref="E20:G20"/>
     <mergeCell ref="C20:D20"/>
     <mergeCell ref="H20:I20"/>
@@ -6415,6 +6349,68 @@
     <mergeCell ref="C22:D22"/>
     <mergeCell ref="H22:I22"/>
     <mergeCell ref="J22:O22"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="J15:O15"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="J16:O16"/>
+    <mergeCell ref="E3:M5"/>
+    <mergeCell ref="C10:O12"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="J14:O14"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="J24:O24"/>
+    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="J17:O17"/>
+    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="J18:O18"/>
+    <mergeCell ref="E19:G19"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="J19:O19"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="J25:O25"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="E27:G27"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="J27:O27"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="J26:O26"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="J28:O28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="E29:G29"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="J29:O29"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="E32:G32"/>
+    <mergeCell ref="H32:I32"/>
+    <mergeCell ref="J32:O32"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="E30:G30"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="J30:O30"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="E31:G31"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="J31:O31"/>
   </mergeCells>
   <conditionalFormatting sqref="C15:O32">
     <cfRule type="expression" dxfId="78" priority="1">
@@ -12908,7 +12904,7 @@
       <selection activeCell="A3" sqref="A3"/>
       <selection pane="topRight" activeCell="E3" sqref="E3"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="A13" sqref="A13"/>
+      <selection pane="bottomRight" activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="6.33203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -19414,7 +19410,7 @@
         <v>1</v>
       </c>
       <c r="J12" s="146">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K12" s="146">
         <v>1</v>
@@ -21083,13 +21079,12 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="IK3:IV4"/>
-    <mergeCell ref="HV3:IJ4"/>
-    <mergeCell ref="EY3:FM4"/>
-    <mergeCell ref="FN3:GB4"/>
-    <mergeCell ref="GC3:GQ4"/>
-    <mergeCell ref="GR3:HF4"/>
-    <mergeCell ref="HG3:HU4"/>
+    <mergeCell ref="EJ3:EX4"/>
+    <mergeCell ref="BM3:CA4"/>
+    <mergeCell ref="CB3:CP4"/>
+    <mergeCell ref="CQ3:DE4"/>
+    <mergeCell ref="DF3:DT4"/>
+    <mergeCell ref="DU3:EI4"/>
     <mergeCell ref="E3:S4"/>
     <mergeCell ref="T3:AH4"/>
     <mergeCell ref="AI3:AW4"/>
@@ -21099,12 +21094,13 @@
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="D5:D6"/>
     <mergeCell ref="A3:D4"/>
-    <mergeCell ref="EJ3:EX4"/>
-    <mergeCell ref="BM3:CA4"/>
-    <mergeCell ref="CB3:CP4"/>
-    <mergeCell ref="CQ3:DE4"/>
-    <mergeCell ref="DF3:DT4"/>
-    <mergeCell ref="DU3:EI4"/>
+    <mergeCell ref="IK3:IV4"/>
+    <mergeCell ref="HV3:IJ4"/>
+    <mergeCell ref="EY3:FM4"/>
+    <mergeCell ref="FN3:GB4"/>
+    <mergeCell ref="GC3:GQ4"/>
+    <mergeCell ref="GR3:HF4"/>
+    <mergeCell ref="HG3:HU4"/>
   </mergeCells>
   <conditionalFormatting sqref="E5:IV6 AQ7:AQ8 AV7:AV8 BA7:BA8 BF7:BF8 BK7:BK8 BP7:BP8 BU7:BU8 BZ7:BZ8 FG7:FG8 GZ7:GZ8 HE7:HE8 HJ7:HJ8 HO7:HO8 HT7:HT8 HY7:HY8 ID7:ID8 II7:II8 IN7:IN8 IS7:IS8 CC7:CC8 N7:N8 FB7:FB8 FL7:FL8 FQ7:FQ8 FV7:FV8 GA7:GA8 GF7:GF8 GK7:GK8 GP7:GP8 GU7:GU8 CE7:CF8 CI7:CJ8 CL7:CL8 CO7:CO8 CR7:CR8 CT7:CU8 CX7:CY8 DA7:DA8 DD7:DE8 DG7:DI8 EG7:EK8 DK7:DL8 EM7:EN8 DN7:DN8 EP7:EP8 DQ7:DQ8 ER7:ES8 DS7:DT8 DV7:DX8 EV7:EX8 DZ7:EA8 EC7:EC8">
     <cfRule type="expression" dxfId="15" priority="143">
@@ -21184,8 +21180,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG41"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="H62" sqref="H62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -21318,7 +21314,7 @@
       </c>
       <c r="I7" s="15">
         <f ca="1">IF($AD7,SUM(INDIRECT(AG7)),"")</f>
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J7" s="22">
         <v>0</v>
@@ -21428,11 +21424,11 @@
       </c>
       <c r="G9" s="15">
         <f ca="1">IF($AD9,INDIRECT($AC9 &amp; "G4"),"")</f>
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H9" s="15">
         <f ca="1">IF($AD9,INDIRECT($AC9 &amp; "D4"),"")</f>
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I9" s="15">
         <f ca="1">IF($AD9,SUM(INDIRECT(AG9)),"")</f>
@@ -21594,15 +21590,15 @@
       <c r="F12" s="179"/>
       <c r="G12" s="109">
         <f ca="1">SUM(G7:G11)</f>
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="H12" s="105">
         <f ca="1">SUM(H7:H11)</f>
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="I12" s="108">
         <f ca="1">SUM(I7:I11)</f>
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="J12" s="110">
         <f>AVERAGE(J7:J11)</f>
@@ -21619,7 +21615,7 @@
       <c r="F14" s="191"/>
       <c r="G14" s="192">
         <f>SUM(Backlog!H:H)</f>
-        <v>452</v>
+        <v>459</v>
       </c>
       <c r="H14" s="192"/>
       <c r="I14" s="192"/>
@@ -21831,9 +21827,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O167"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="C1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H42" sqref="H42"/>
+    <sheetView showGridLines="0" topLeftCell="D1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <pane ySplit="5" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H76" sqref="H76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -22416,7 +22412,7 @@
         <v>5</v>
       </c>
       <c r="H16" s="141">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I16" s="142" t="s">
         <v>171</v>
@@ -22455,7 +22451,7 @@
         <v>1.3.2</v>
       </c>
       <c r="F17" s="143">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G17" s="143">
         <v>5</v>
@@ -22551,7 +22547,7 @@
         <v>4</v>
       </c>
       <c r="H19" s="141">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="I19" s="142" t="s">
         <v>62</v>
@@ -23721,7 +23717,7 @@
         <v>3</v>
       </c>
       <c r="H45" s="141">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I45" s="142" t="s">
         <v>211</v>
@@ -24660,7 +24656,7 @@
         <v>4.3.2</v>
       </c>
       <c r="F66" s="143">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G66" s="143">
         <v>6</v>
@@ -25206,7 +25202,7 @@
         <v>5</v>
       </c>
       <c r="H78" s="141">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I78" s="142" t="s">
         <v>74</v>
@@ -25251,7 +25247,7 @@
         <v>6</v>
       </c>
       <c r="H79" s="141">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I79" s="142" t="s">
         <v>74</v>
@@ -29174,8 +29170,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CE55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B3" zoomScale="70" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView topLeftCell="B3" zoomScale="70" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="J65" sqref="J65:K66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -41747,7 +41743,7 @@
   <dimension ref="A1:CE47"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <pane xSplit="7" ySplit="6" topLeftCell="N7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="6" topLeftCell="H7" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
@@ -42667,7 +42663,7 @@
       <c r="C4" s="209"/>
       <c r="D4" s="72">
         <f ca="1">IF(AND(TODAY()&gt;=F3,TODAY()&lt;=F4),INDIRECT(ADDRESS(6,7+MATCH(TODAY(),H4:BZ4,0))),IF(TODAY()&lt;F3,G4,0))</f>
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E4" s="86" t="s">
         <v>10</v>
@@ -42677,7 +42673,7 @@
       </c>
       <c r="G4" s="63">
         <f ca="1">SUM(G7:G42)</f>
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H4" s="25">
         <f>H3</f>
@@ -42992,79 +42988,79 @@
       </c>
       <c r="H5" s="124">
         <f ca="1">G4</f>
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I5" s="82">
         <f ca="1">IF(I2,H5-$H$5/$F$2,"")</f>
-        <v>76.73684210526315</v>
+        <v>75.78947368421052</v>
       </c>
       <c r="J5" s="82">
         <f t="shared" ref="J5:BU5" ca="1" si="5">IF(J2,I5-$H$5/$F$2,"")</f>
-        <v>72.473684210526301</v>
+        <v>71.578947368421041</v>
       </c>
       <c r="K5" s="82">
         <f t="shared" ca="1" si="5"/>
-        <v>68.210526315789451</v>
+        <v>67.368421052631561</v>
       </c>
       <c r="L5" s="82">
         <f t="shared" ca="1" si="5"/>
-        <v>63.947368421052609</v>
+        <v>63.157894736842088</v>
       </c>
       <c r="M5" s="82">
         <f t="shared" ca="1" si="5"/>
-        <v>59.684210526315766</v>
+        <v>58.947368421052616</v>
       </c>
       <c r="N5" s="82">
         <f t="shared" ca="1" si="5"/>
-        <v>55.421052631578924</v>
+        <v>54.736842105263143</v>
       </c>
       <c r="O5" s="82">
         <f t="shared" ca="1" si="5"/>
-        <v>51.157894736842081</v>
+        <v>50.526315789473671</v>
       </c>
       <c r="P5" s="82">
         <f t="shared" ca="1" si="5"/>
-        <v>46.894736842105239</v>
+        <v>46.315789473684198</v>
       </c>
       <c r="Q5" s="82">
         <f t="shared" ca="1" si="5"/>
-        <v>42.631578947368396</v>
+        <v>42.105263157894726</v>
       </c>
       <c r="R5" s="82">
         <f t="shared" ca="1" si="5"/>
-        <v>38.368421052631554</v>
+        <v>37.894736842105253</v>
       </c>
       <c r="S5" s="82">
         <f t="shared" ca="1" si="5"/>
-        <v>34.105263157894711</v>
+        <v>33.68421052631578</v>
       </c>
       <c r="T5" s="82">
         <f t="shared" ca="1" si="5"/>
-        <v>29.842105263157869</v>
+        <v>29.473684210526308</v>
       </c>
       <c r="U5" s="82">
         <f t="shared" ca="1" si="5"/>
-        <v>25.578947368421026</v>
+        <v>25.263157894736835</v>
       </c>
       <c r="V5" s="82">
         <f t="shared" ca="1" si="5"/>
-        <v>21.315789473684184</v>
+        <v>21.052631578947363</v>
       </c>
       <c r="W5" s="82">
         <f t="shared" ca="1" si="5"/>
-        <v>17.052631578947341</v>
+        <v>16.84210526315789</v>
       </c>
       <c r="X5" s="82">
         <f t="shared" ca="1" si="5"/>
-        <v>12.789473684210499</v>
+        <v>12.631578947368418</v>
       </c>
       <c r="Y5" s="82">
         <f t="shared" ca="1" si="5"/>
-        <v>8.5263157894736565</v>
+        <v>8.4210526315789451</v>
       </c>
       <c r="Z5" s="82">
         <f t="shared" ca="1" si="5"/>
-        <v>4.2631578947368141</v>
+        <v>4.2105263157894717</v>
       </c>
       <c r="AA5" s="44" t="str">
         <f t="shared" si="5"/>
@@ -43620,7 +43616,7 @@
       </c>
       <c r="G7" s="66">
         <f ca="1">IF($B7="","",INDEX(Backlog!$A:$M,$A7,G$5))</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H7" s="26"/>
       <c r="I7" s="26"/>
@@ -43717,31 +43713,31 @@
     <row r="8" spans="1:83" ht="26">
       <c r="A8" s="90">
         <f t="shared" ref="A8:A42" ca="1" si="10">CA8-1</f>
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B8" s="18" t="str">
         <f ca="1">IF(ISNUMBER(A8),INDEX(Backlog!$A:$M,$A8,B$5),"")</f>
-        <v>1.3.2</v>
+        <v>2.1.2</v>
       </c>
       <c r="C8" s="73" t="str">
         <f ca="1">IF($B8="","",INDEX(Backlog!$A:$M,$A8,C$5))</f>
-        <v>BackOffice WebServices</v>
+        <v>BackOffice</v>
       </c>
       <c r="D8" s="73" t="str">
         <f ca="1">IF($B8="","",INDEX(Backlog!$A:$M,$A8,D$5))</f>
-        <v>WS Post</v>
+        <v>I18n</v>
       </c>
       <c r="E8" s="73" t="str">
         <f ca="1">IF($B8="","",INDEX(Backlog!$A:$M,$A8,E$5))</f>
-        <v>Creation de Parcours</v>
+        <v>Modification "Core"</v>
       </c>
       <c r="F8" s="48">
         <f ca="1">IF($B8="","",INDEX(Backlog!$A:$M,$A8,F$5))</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G8" s="66">
         <f ca="1">IF($B8="","",INDEX(Backlog!$A:$M,$A8,G$5))</f>
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="H8" s="26"/>
       <c r="I8" s="26"/>
@@ -43816,7 +43812,7 @@
       <c r="BZ8" s="84"/>
       <c r="CA8" s="21">
         <f ca="1">IF($CE8="","",CE8)</f>
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="CB8" s="21">
         <f t="shared" ca="1" si="7"/>
@@ -43824,25 +43820,25 @@
       </c>
       <c r="CC8" s="21" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>Backlog!$F$18:$F$151</v>
+        <v>Backlog!$F$20:$F$151</v>
       </c>
       <c r="CD8" s="21">
         <f t="shared" ca="1" si="9"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="CE8" s="21">
         <f ca="1">IF(ISNA($CD8),"",CE7+CD8)</f>
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:83">
       <c r="A9" s="90">
         <f t="shared" ca="1" si="10"/>
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B9" s="18" t="str">
         <f ca="1">IF(ISNUMBER(A9),INDEX(Backlog!$A:$M,$A9,B$5),"")</f>
-        <v>2.1.2</v>
+        <v>2.2.1</v>
       </c>
       <c r="C9" s="73" t="str">
         <f ca="1">IF($B9="","",INDEX(Backlog!$A:$M,$A9,C$5))</f>
@@ -43850,11 +43846,11 @@
       </c>
       <c r="D9" s="73" t="str">
         <f ca="1">IF($B9="","",INDEX(Backlog!$A:$M,$A9,D$5))</f>
-        <v>I18n</v>
+        <v>Historique Consultation</v>
       </c>
       <c r="E9" s="73" t="str">
         <f ca="1">IF($B9="","",INDEX(Backlog!$A:$M,$A9,E$5))</f>
-        <v>Modification "Core"</v>
+        <v>Architecture BDD</v>
       </c>
       <c r="F9" s="48">
         <f ca="1">IF($B9="","",INDEX(Backlog!$A:$M,$A9,F$5))</f>
@@ -43862,7 +43858,7 @@
       </c>
       <c r="G9" s="66">
         <f ca="1">IF($B9="","",INDEX(Backlog!$A:$M,$A9,G$5))</f>
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="H9" s="26"/>
       <c r="I9" s="26"/>
@@ -43937,7 +43933,7 @@
       <c r="BZ9" s="84"/>
       <c r="CA9" s="21">
         <f ca="1">IF($CE9="","",CE9)</f>
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="CB9" s="21">
         <f t="shared" ca="1" si="7"/>
@@ -43945,25 +43941,25 @@
       </c>
       <c r="CC9" s="21" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>Backlog!$F$20:$F$151</v>
+        <v>Backlog!$F$23:$F$151</v>
       </c>
       <c r="CD9" s="21">
         <f t="shared" ca="1" si="9"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="CE9" s="21">
         <f ca="1">IF(ISNA($CD9),"",CE8+CD9)</f>
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:83">
       <c r="A10" s="90">
         <f t="shared" ca="1" si="10"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B10" s="18" t="str">
         <f ca="1">IF(ISNUMBER(A10),INDEX(Backlog!$A:$M,$A10,B$5),"")</f>
-        <v>2.2.1</v>
+        <v>2.2.2</v>
       </c>
       <c r="C10" s="73" t="str">
         <f ca="1">IF($B10="","",INDEX(Backlog!$A:$M,$A10,C$5))</f>
@@ -43975,7 +43971,7 @@
       </c>
       <c r="E10" s="73" t="str">
         <f ca="1">IF($B10="","",INDEX(Backlog!$A:$M,$A10,E$5))</f>
-        <v>Architecture BDD</v>
+        <v>Modification WS</v>
       </c>
       <c r="F10" s="48">
         <f ca="1">IF($B10="","",INDEX(Backlog!$A:$M,$A10,F$5))</f>
@@ -44058,7 +44054,7 @@
       <c r="BZ10" s="84"/>
       <c r="CA10" s="21">
         <f ca="1">IF($CE10="","",CE10)</f>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="CB10" s="21">
         <f t="shared" ca="1" si="7"/>
@@ -44066,25 +44062,25 @@
       </c>
       <c r="CC10" s="21" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>Backlog!$F$23:$F$151</v>
+        <v>Backlog!$F$24:$F$151</v>
       </c>
       <c r="CD10" s="21">
         <f t="shared" ca="1" si="9"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="CE10" s="21">
         <f ca="1">IF(ISNA($CD10),"",CE9+CD10)</f>
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:83">
       <c r="A11" s="90">
         <f t="shared" ca="1" si="10"/>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B11" s="18" t="str">
         <f ca="1">IF(ISNUMBER(A11),INDEX(Backlog!$A:$M,$A11,B$5),"")</f>
-        <v>2.2.2</v>
+        <v>2.2.3</v>
       </c>
       <c r="C11" s="73" t="str">
         <f ca="1">IF($B11="","",INDEX(Backlog!$A:$M,$A11,C$5))</f>
@@ -44096,7 +44092,7 @@
       </c>
       <c r="E11" s="73" t="str">
         <f ca="1">IF($B11="","",INDEX(Backlog!$A:$M,$A11,E$5))</f>
-        <v>Modification WS</v>
+        <v>Creation WS getHistoriqueByUserId (+modif WSDL)</v>
       </c>
       <c r="F11" s="48">
         <f ca="1">IF($B11="","",INDEX(Backlog!$A:$M,$A11,F$5))</f>
@@ -44179,7 +44175,7 @@
       <c r="BZ11" s="84"/>
       <c r="CA11" s="21">
         <f t="shared" ref="CA11:CA42" ca="1" si="11">IF($CE11="","",CE11)</f>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="CB11" s="21">
         <f t="shared" ca="1" si="7"/>
@@ -44187,7 +44183,7 @@
       </c>
       <c r="CC11" s="21" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>Backlog!$F$24:$F$151</v>
+        <v>Backlog!$F$25:$F$151</v>
       </c>
       <c r="CD11" s="21">
         <f t="shared" ca="1" si="9"/>
@@ -44195,33 +44191,33 @@
       </c>
       <c r="CE11" s="21">
         <f t="shared" ref="CE11:CE42" ca="1" si="12">IF(ISNA($CD11),"",CE10+CD11)</f>
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:83">
       <c r="A12" s="90">
         <f t="shared" ca="1" si="10"/>
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="B12" s="18" t="str">
         <f ca="1">IF(ISNUMBER(A12),INDEX(Backlog!$A:$M,$A12,B$5),"")</f>
-        <v>2.2.3</v>
+        <v>3.2.1</v>
       </c>
       <c r="C12" s="73" t="str">
         <f ca="1">IF($B12="","",INDEX(Backlog!$A:$M,$A12,C$5))</f>
-        <v>BackOffice</v>
+        <v>LinkServer (LS)</v>
       </c>
       <c r="D12" s="73" t="str">
         <f ca="1">IF($B12="","",INDEX(Backlog!$A:$M,$A12,D$5))</f>
-        <v>Historique Consultation</v>
+        <v>IHM</v>
       </c>
       <c r="E12" s="73" t="str">
         <f ca="1">IF($B12="","",INDEX(Backlog!$A:$M,$A12,E$5))</f>
-        <v>Creation WS getHistoriqueByUserId (+modif WSDL)</v>
+        <v>Interface Admin CRUD</v>
       </c>
       <c r="F12" s="48">
         <f ca="1">IF($B12="","",INDEX(Backlog!$A:$M,$A12,F$5))</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G12" s="66">
         <f ca="1">IF($B12="","",INDEX(Backlog!$A:$M,$A12,G$5))</f>
@@ -44300,7 +44296,7 @@
       <c r="BZ12" s="84"/>
       <c r="CA12" s="21">
         <f t="shared" ca="1" si="11"/>
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="CB12" s="21">
         <f t="shared" ca="1" si="7"/>
@@ -44308,25 +44304,25 @@
       </c>
       <c r="CC12" s="21" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>Backlog!$F$25:$F$151</v>
+        <v>Backlog!$F$45:$F$151</v>
       </c>
       <c r="CD12" s="21">
         <f t="shared" ca="1" si="9"/>
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="CE12" s="21">
         <f t="shared" ca="1" si="12"/>
-        <v>25</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:83">
       <c r="A13" s="90">
         <f t="shared" ca="1" si="10"/>
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B13" s="18" t="str">
         <f ca="1">IF(ISNUMBER(A13),INDEX(Backlog!$A:$M,$A13,B$5),"")</f>
-        <v>3.2.1</v>
+        <v>3.2.2</v>
       </c>
       <c r="C13" s="73" t="str">
         <f ca="1">IF($B13="","",INDEX(Backlog!$A:$M,$A13,C$5))</f>
@@ -44338,7 +44334,7 @@
       </c>
       <c r="E13" s="73" t="str">
         <f ca="1">IF($B13="","",INDEX(Backlog!$A:$M,$A13,E$5))</f>
-        <v>Interface Admin CRUD</v>
+        <v>Interface Admin GPS (V1 : juste pts central + rayon)</v>
       </c>
       <c r="F13" s="48">
         <f ca="1">IF($B13="","",INDEX(Backlog!$A:$M,$A13,F$5))</f>
@@ -44346,7 +44342,7 @@
       </c>
       <c r="G13" s="66">
         <f ca="1">IF($B13="","",INDEX(Backlog!$A:$M,$A13,G$5))</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H13" s="26"/>
       <c r="I13" s="26"/>
@@ -44421,7 +44417,7 @@
       <c r="BZ13" s="84"/>
       <c r="CA13" s="21">
         <f t="shared" ca="1" si="11"/>
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="CB13" s="21">
         <f t="shared" ca="1" si="7"/>
@@ -44429,25 +44425,25 @@
       </c>
       <c r="CC13" s="21" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>Backlog!$F$45:$F$151</v>
+        <v>Backlog!$F$46:$F$151</v>
       </c>
       <c r="CD13" s="21">
         <f t="shared" ca="1" si="9"/>
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="CE13" s="21">
         <f t="shared" ca="1" si="12"/>
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:83">
       <c r="A14" s="90">
         <f t="shared" ca="1" si="10"/>
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B14" s="18" t="str">
         <f ca="1">IF(ISNUMBER(A14),INDEX(Backlog!$A:$M,$A14,B$5),"")</f>
-        <v>3.2.2</v>
+        <v>3.3.2</v>
       </c>
       <c r="C14" s="73" t="str">
         <f ca="1">IF($B14="","",INDEX(Backlog!$A:$M,$A14,C$5))</f>
@@ -44455,19 +44451,19 @@
       </c>
       <c r="D14" s="73" t="str">
         <f ca="1">IF($B14="","",INDEX(Backlog!$A:$M,$A14,D$5))</f>
-        <v>IHM</v>
+        <v>WS Read</v>
       </c>
       <c r="E14" s="73" t="str">
         <f ca="1">IF($B14="","",INDEX(Backlog!$A:$M,$A14,E$5))</f>
-        <v>Interface Admin GPS (V1 : juste pts central + rayon)</v>
+        <v>Fonction getSceneByGPSCoord / getSceneByGPSCoord  (V1 : juste pts central + rayon)</v>
       </c>
       <c r="F14" s="48">
         <f ca="1">IF($B14="","",INDEX(Backlog!$A:$M,$A14,F$5))</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G14" s="66">
         <f ca="1">IF($B14="","",INDEX(Backlog!$A:$M,$A14,G$5))</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H14" s="26"/>
       <c r="I14" s="26"/>
@@ -44542,7 +44538,7 @@
       <c r="BZ14" s="84"/>
       <c r="CA14" s="21">
         <f t="shared" ca="1" si="11"/>
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="CB14" s="21">
         <f t="shared" ca="1" si="7"/>
@@ -44550,25 +44546,25 @@
       </c>
       <c r="CC14" s="21" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>Backlog!$F$46:$F$151</v>
+        <v>Backlog!$F$49:$F$151</v>
       </c>
       <c r="CD14" s="21">
         <f t="shared" ca="1" si="9"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="CE14" s="21">
         <f t="shared" ca="1" si="12"/>
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:83">
       <c r="A15" s="90">
         <f t="shared" ca="1" si="10"/>
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B15" s="18" t="str">
         <f ca="1">IF(ISNUMBER(A15),INDEX(Backlog!$A:$M,$A15,B$5),"")</f>
-        <v>3.3.2</v>
+        <v>3.4.1</v>
       </c>
       <c r="C15" s="73" t="str">
         <f ca="1">IF($B15="","",INDEX(Backlog!$A:$M,$A15,C$5))</f>
@@ -44576,15 +44572,15 @@
       </c>
       <c r="D15" s="73" t="str">
         <f ca="1">IF($B15="","",INDEX(Backlog!$A:$M,$A15,D$5))</f>
-        <v>WS Read</v>
+        <v>WS Post</v>
       </c>
       <c r="E15" s="73" t="str">
         <f ca="1">IF($B15="","",INDEX(Backlog!$A:$M,$A15,E$5))</f>
-        <v>Fonction getSceneByGPSCoord / getSceneByGPSCoord  (V1 : juste pts central + rayon)</v>
+        <v>Fonction postLinkTagScene</v>
       </c>
       <c r="F15" s="48">
         <f ca="1">IF($B15="","",INDEX(Backlog!$A:$M,$A15,F$5))</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G15" s="66">
         <f ca="1">IF($B15="","",INDEX(Backlog!$A:$M,$A15,G$5))</f>
@@ -44663,7 +44659,7 @@
       <c r="BZ15" s="84"/>
       <c r="CA15" s="21">
         <f t="shared" ca="1" si="11"/>
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="CB15" s="21">
         <f t="shared" ca="1" si="7"/>
@@ -44671,25 +44667,25 @@
       </c>
       <c r="CC15" s="21" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>Backlog!$F$49:$F$151</v>
+        <v>Backlog!$F$51:$F$151</v>
       </c>
       <c r="CD15" s="21">
         <f t="shared" ca="1" si="9"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="CE15" s="21">
         <f t="shared" ca="1" si="12"/>
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:83">
       <c r="A16" s="90">
         <f t="shared" ca="1" si="10"/>
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B16" s="18" t="str">
         <f ca="1">IF(ISNUMBER(A16),INDEX(Backlog!$A:$M,$A16,B$5),"")</f>
-        <v>3.4.1</v>
+        <v>3.4.2</v>
       </c>
       <c r="C16" s="73" t="str">
         <f ca="1">IF($B16="","",INDEX(Backlog!$A:$M,$A16,C$5))</f>
@@ -44701,7 +44697,7 @@
       </c>
       <c r="E16" s="73" t="str">
         <f ca="1">IF($B16="","",INDEX(Backlog!$A:$M,$A16,E$5))</f>
-        <v>Fonction postLinkTagScene</v>
+        <v>Fonction postLinkGPSCoordScene (V1 : juste pts central + rayon)</v>
       </c>
       <c r="F16" s="48">
         <f ca="1">IF($B16="","",INDEX(Backlog!$A:$M,$A16,F$5))</f>
@@ -44784,7 +44780,7 @@
       <c r="BZ16" s="84"/>
       <c r="CA16" s="21">
         <f t="shared" ca="1" si="11"/>
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="CB16" s="21">
         <f t="shared" ca="1" si="7"/>
@@ -44792,41 +44788,41 @@
       </c>
       <c r="CC16" s="21" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>Backlog!$F$51:$F$151</v>
+        <v>Backlog!$F$52:$F$151</v>
       </c>
       <c r="CD16" s="21">
         <f t="shared" ca="1" si="9"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="CE16" s="21">
         <f t="shared" ca="1" si="12"/>
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:83">
       <c r="A17" s="90">
         <f t="shared" ca="1" si="10"/>
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="B17" s="18" t="str">
         <f ca="1">IF(ISNUMBER(A17),INDEX(Backlog!$A:$M,$A17,B$5),"")</f>
-        <v>3.4.2</v>
+        <v>4.2.8</v>
       </c>
       <c r="C17" s="73" t="str">
         <f ca="1">IF($B17="","",INDEX(Backlog!$A:$M,$A17,C$5))</f>
-        <v>LinkServer (LS)</v>
+        <v>API Java BO</v>
       </c>
       <c r="D17" s="73" t="str">
         <f ca="1">IF($B17="","",INDEX(Backlog!$A:$M,$A17,D$5))</f>
-        <v>WS Post</v>
+        <v>API Java BO : Read</v>
       </c>
       <c r="E17" s="73" t="str">
         <f ca="1">IF($B17="","",INDEX(Backlog!$A:$M,$A17,E$5))</f>
-        <v>Fonction postLinkGPSCoordScene (V1 : juste pts central + rayon)</v>
+        <v>Fonction getHistoriqueByUserId</v>
       </c>
       <c r="F17" s="48">
         <f ca="1">IF($B17="","",INDEX(Backlog!$A:$M,$A17,F$5))</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G17" s="66">
         <f ca="1">IF($B17="","",INDEX(Backlog!$A:$M,$A17,G$5))</f>
@@ -44905,7 +44901,7 @@
       <c r="BZ17" s="84"/>
       <c r="CA17" s="21">
         <f t="shared" ca="1" si="11"/>
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="CB17" s="21">
         <f t="shared" ca="1" si="7"/>
@@ -44913,25 +44909,25 @@
       </c>
       <c r="CC17" s="21" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>Backlog!$F$52:$F$151</v>
+        <v>Backlog!$F$63:$F$151</v>
       </c>
       <c r="CD17" s="21">
         <f t="shared" ca="1" si="9"/>
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="CE17" s="21">
         <f t="shared" ca="1" si="12"/>
-        <v>52</v>
+        <v>63</v>
       </c>
     </row>
     <row r="18" spans="1:83">
       <c r="A18" s="90">
         <f t="shared" ca="1" si="10"/>
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B18" s="18" t="str">
         <f ca="1">IF(ISNUMBER(A18),INDEX(Backlog!$A:$M,$A18,B$5),"")</f>
-        <v>4.2.8</v>
+        <v>4.3.1</v>
       </c>
       <c r="C18" s="73" t="str">
         <f ca="1">IF($B18="","",INDEX(Backlog!$A:$M,$A18,C$5))</f>
@@ -44939,19 +44935,19 @@
       </c>
       <c r="D18" s="73" t="str">
         <f ca="1">IF($B18="","",INDEX(Backlog!$A:$M,$A18,D$5))</f>
-        <v>API Java BO : Read</v>
+        <v>API Java BO : Post</v>
       </c>
       <c r="E18" s="73" t="str">
         <f ca="1">IF($B18="","",INDEX(Backlog!$A:$M,$A18,E$5))</f>
-        <v>Fonction getHistoriqueByUserId</v>
+        <v>Fonction Post Media (Lié à rien / à une scène / à une artefact)</v>
       </c>
       <c r="F18" s="48">
         <f ca="1">IF($B18="","",INDEX(Backlog!$A:$M,$A18,F$5))</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G18" s="66">
         <f ca="1">IF($B18="","",INDEX(Backlog!$A:$M,$A18,G$5))</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H18" s="26"/>
       <c r="I18" s="26"/>
@@ -45026,7 +45022,7 @@
       <c r="BZ18" s="84"/>
       <c r="CA18" s="21">
         <f t="shared" ca="1" si="11"/>
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="CB18" s="21">
         <f t="shared" ca="1" si="7"/>
@@ -45034,45 +45030,45 @@
       </c>
       <c r="CC18" s="21" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>Backlog!$F$63:$F$151</v>
+        <v>Backlog!$F$66:$F$151</v>
       </c>
       <c r="CD18" s="21">
         <f t="shared" ca="1" si="9"/>
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="CE18" s="21">
         <f t="shared" ca="1" si="12"/>
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="19" spans="1:83">
       <c r="A19" s="90">
         <f t="shared" ca="1" si="10"/>
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="B19" s="18" t="str">
         <f ca="1">IF(ISNUMBER(A19),INDEX(Backlog!$A:$M,$A19,B$5),"")</f>
-        <v>4.3.1</v>
+        <v>5.3.1</v>
       </c>
       <c r="C19" s="73" t="str">
         <f ca="1">IF($B19="","",INDEX(Backlog!$A:$M,$A19,C$5))</f>
-        <v>API Java BO</v>
+        <v>API Java LS</v>
       </c>
       <c r="D19" s="73" t="str">
         <f ca="1">IF($B19="","",INDEX(Backlog!$A:$M,$A19,D$5))</f>
-        <v>API Java BO : Post</v>
+        <v>API Java LS : Post</v>
       </c>
       <c r="E19" s="73" t="str">
         <f ca="1">IF($B19="","",INDEX(Backlog!$A:$M,$A19,E$5))</f>
-        <v>Fonction Post Media (Lié à rien / à une scène / à une artefact)</v>
+        <v>Fonction postLinkTagScene</v>
       </c>
       <c r="F19" s="48">
         <f ca="1">IF($B19="","",INDEX(Backlog!$A:$M,$A19,F$5))</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G19" s="66">
         <f ca="1">IF($B19="","",INDEX(Backlog!$A:$M,$A19,G$5))</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H19" s="26"/>
       <c r="I19" s="26"/>
@@ -45147,7 +45143,7 @@
       <c r="BZ19" s="84"/>
       <c r="CA19" s="21">
         <f t="shared" ca="1" si="11"/>
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="CB19" s="21">
         <f t="shared" ca="1" si="7"/>
@@ -45155,45 +45151,45 @@
       </c>
       <c r="CC19" s="21" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>Backlog!$F$66:$F$151</v>
+        <v>Backlog!$F$71:$F$151</v>
       </c>
       <c r="CD19" s="21">
         <f t="shared" ca="1" si="9"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="CE19" s="21">
         <f t="shared" ca="1" si="12"/>
-        <v>66</v>
+        <v>71</v>
       </c>
     </row>
     <row r="20" spans="1:83">
       <c r="A20" s="90">
         <f t="shared" ca="1" si="10"/>
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="B20" s="18" t="str">
         <f ca="1">IF(ISNUMBER(A20),INDEX(Backlog!$A:$M,$A20,B$5),"")</f>
-        <v>4.3.2</v>
+        <v>5.3.2</v>
       </c>
       <c r="C20" s="73" t="str">
         <f ca="1">IF($B20="","",INDEX(Backlog!$A:$M,$A20,C$5))</f>
-        <v>API Java BO</v>
+        <v>API Java LS</v>
       </c>
       <c r="D20" s="73" t="str">
         <f ca="1">IF($B20="","",INDEX(Backlog!$A:$M,$A20,D$5))</f>
-        <v>API Java BO : Post</v>
+        <v>API Java LS : Post</v>
       </c>
       <c r="E20" s="73" t="str">
         <f ca="1">IF($B20="","",INDEX(Backlog!$A:$M,$A20,E$5))</f>
-        <v>Creation de Parcours</v>
+        <v>Fonction postLinkGPSCoordScene  (V1 : juste pts central + rayon)</v>
       </c>
       <c r="F20" s="48">
         <f ca="1">IF($B20="","",INDEX(Backlog!$A:$M,$A20,F$5))</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G20" s="66">
         <f ca="1">IF($B20="","",INDEX(Backlog!$A:$M,$A20,G$5))</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H20" s="26"/>
       <c r="I20" s="26"/>
@@ -45268,7 +45264,7 @@
       <c r="BZ20" s="84"/>
       <c r="CA20" s="21">
         <f t="shared" ca="1" si="11"/>
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="CB20" s="21">
         <f t="shared" ca="1" si="7"/>
@@ -45276,7 +45272,7 @@
       </c>
       <c r="CC20" s="21" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>Backlog!$F$67:$F$151</v>
+        <v>Backlog!$F$72:$F$151</v>
       </c>
       <c r="CD20" s="21">
         <f t="shared" ca="1" si="9"/>
@@ -45284,29 +45280,29 @@
       </c>
       <c r="CE20" s="21">
         <f t="shared" ca="1" si="12"/>
-        <v>67</v>
+        <v>72</v>
       </c>
     </row>
     <row r="21" spans="1:83">
       <c r="A21" s="90">
         <f t="shared" ca="1" si="10"/>
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="B21" s="18" t="str">
         <f ca="1">IF(ISNUMBER(A21),INDEX(Backlog!$A:$M,$A21,B$5),"")</f>
-        <v>5.3.1</v>
+        <v>6.1.3</v>
       </c>
       <c r="C21" s="73" t="str">
         <f ca="1">IF($B21="","",INDEX(Backlog!$A:$M,$A21,C$5))</f>
-        <v>API Java LS</v>
+        <v>Android</v>
       </c>
       <c r="D21" s="73" t="str">
         <f ca="1">IF($B21="","",INDEX(Backlog!$A:$M,$A21,D$5))</f>
-        <v>API Java LS : Post</v>
+        <v>Capteurs</v>
       </c>
       <c r="E21" s="73" t="str">
         <f ca="1">IF($B21="","",INDEX(Backlog!$A:$M,$A21,E$5))</f>
-        <v>Fonction postLinkTagScene</v>
+        <v>Lire les coordonnées GPS</v>
       </c>
       <c r="F21" s="48">
         <f ca="1">IF($B21="","",INDEX(Backlog!$A:$M,$A21,F$5))</f>
@@ -45314,7 +45310,7 @@
       </c>
       <c r="G21" s="66">
         <f ca="1">IF($B21="","",INDEX(Backlog!$A:$M,$A21,G$5))</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H21" s="26"/>
       <c r="I21" s="26"/>
@@ -45389,7 +45385,7 @@
       <c r="BZ21" s="84"/>
       <c r="CA21" s="21">
         <f t="shared" ca="1" si="11"/>
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="CB21" s="21">
         <f t="shared" ca="1" si="7"/>
@@ -45397,7 +45393,7 @@
       </c>
       <c r="CC21" s="21" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>Backlog!$F$71:$F$151</v>
+        <v>Backlog!$F$76:$F$151</v>
       </c>
       <c r="CD21" s="21">
         <f t="shared" ca="1" si="9"/>
@@ -45405,29 +45401,29 @@
       </c>
       <c r="CE21" s="21">
         <f t="shared" ca="1" si="12"/>
-        <v>71</v>
+        <v>76</v>
       </c>
     </row>
     <row r="22" spans="1:83">
       <c r="A22" s="90">
         <f t="shared" ca="1" si="10"/>
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="B22" s="18" t="str">
         <f ca="1">IF(ISNUMBER(A22),INDEX(Backlog!$A:$M,$A22,B$5),"")</f>
-        <v>5.3.2</v>
+        <v>6.1.4</v>
       </c>
       <c r="C22" s="73" t="str">
         <f ca="1">IF($B22="","",INDEX(Backlog!$A:$M,$A22,C$5))</f>
-        <v>API Java LS</v>
+        <v>Android</v>
       </c>
       <c r="D22" s="73" t="str">
         <f ca="1">IF($B22="","",INDEX(Backlog!$A:$M,$A22,D$5))</f>
-        <v>API Java LS : Post</v>
+        <v>Capteurs</v>
       </c>
       <c r="E22" s="73" t="str">
         <f ca="1">IF($B22="","",INDEX(Backlog!$A:$M,$A22,E$5))</f>
-        <v>Fonction postLinkGPSCoordScene  (V1 : juste pts central + rayon)</v>
+        <v>Gestion de modes</v>
       </c>
       <c r="F22" s="48">
         <f ca="1">IF($B22="","",INDEX(Backlog!$A:$M,$A22,F$5))</f>
@@ -45435,7 +45431,7 @@
       </c>
       <c r="G22" s="66">
         <f ca="1">IF($B22="","",INDEX(Backlog!$A:$M,$A22,G$5))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H22" s="26"/>
       <c r="I22" s="26"/>
@@ -45510,7 +45506,7 @@
       <c r="BZ22" s="84"/>
       <c r="CA22" s="21">
         <f t="shared" ca="1" si="11"/>
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="CB22" s="21">
         <f t="shared" ca="1" si="7"/>
@@ -45518,7 +45514,7 @@
       </c>
       <c r="CC22" s="21" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>Backlog!$F$72:$F$151</v>
+        <v>Backlog!$F$77:$F$151</v>
       </c>
       <c r="CD22" s="21">
         <f t="shared" ca="1" si="9"/>
@@ -45526,17 +45522,17 @@
       </c>
       <c r="CE22" s="21">
         <f t="shared" ca="1" si="12"/>
-        <v>72</v>
+        <v>77</v>
       </c>
     </row>
     <row r="23" spans="1:83">
       <c r="A23" s="90">
         <f t="shared" ca="1" si="10"/>
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B23" s="18" t="str">
         <f ca="1">IF(ISNUMBER(A23),INDEX(Backlog!$A:$M,$A23,B$5),"")</f>
-        <v>6.1.3</v>
+        <v>6.1.5</v>
       </c>
       <c r="C23" s="73" t="str">
         <f ca="1">IF($B23="","",INDEX(Backlog!$A:$M,$A23,C$5))</f>
@@ -45548,7 +45544,7 @@
       </c>
       <c r="E23" s="73" t="str">
         <f ca="1">IF($B23="","",INDEX(Backlog!$A:$M,$A23,E$5))</f>
-        <v>Lire les coordonnées GPS</v>
+        <v>Mode intérieur</v>
       </c>
       <c r="F23" s="48">
         <f ca="1">IF($B23="","",INDEX(Backlog!$A:$M,$A23,F$5))</f>
@@ -45556,7 +45552,7 @@
       </c>
       <c r="G23" s="66">
         <f ca="1">IF($B23="","",INDEX(Backlog!$A:$M,$A23,G$5))</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H23" s="26"/>
       <c r="I23" s="26"/>
@@ -45631,7 +45627,7 @@
       <c r="BZ23" s="84"/>
       <c r="CA23" s="21">
         <f t="shared" ca="1" si="11"/>
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="CB23" s="21">
         <f t="shared" ca="1" si="7"/>
@@ -45639,25 +45635,25 @@
       </c>
       <c r="CC23" s="21" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>Backlog!$F$76:$F$151</v>
+        <v>Backlog!$F$78:$F$151</v>
       </c>
       <c r="CD23" s="21">
         <f t="shared" ca="1" si="9"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="CE23" s="21">
         <f t="shared" ca="1" si="12"/>
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="24" spans="1:83">
       <c r="A24" s="90">
         <f t="shared" ca="1" si="10"/>
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B24" s="18" t="str">
         <f ca="1">IF(ISNUMBER(A24),INDEX(Backlog!$A:$M,$A24,B$5),"")</f>
-        <v>6.1.4</v>
+        <v>6.1.6</v>
       </c>
       <c r="C24" s="73" t="str">
         <f ca="1">IF($B24="","",INDEX(Backlog!$A:$M,$A24,C$5))</f>
@@ -45669,7 +45665,7 @@
       </c>
       <c r="E24" s="73" t="str">
         <f ca="1">IF($B24="","",INDEX(Backlog!$A:$M,$A24,E$5))</f>
-        <v>Gestion de modes</v>
+        <v>Mode extérieur</v>
       </c>
       <c r="F24" s="48">
         <f ca="1">IF($B24="","",INDEX(Backlog!$A:$M,$A24,F$5))</f>
@@ -45752,7 +45748,7 @@
       <c r="BZ24" s="84"/>
       <c r="CA24" s="21">
         <f t="shared" ca="1" si="11"/>
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="CB24" s="21">
         <f t="shared" ca="1" si="7"/>
@@ -45760,7 +45756,7 @@
       </c>
       <c r="CC24" s="21" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>Backlog!$F$77:$F$151</v>
+        <v>Backlog!$F$79:$F$151</v>
       </c>
       <c r="CD24" s="21">
         <f t="shared" ca="1" si="9"/>
@@ -45768,17 +45764,17 @@
       </c>
       <c r="CE24" s="21">
         <f t="shared" ca="1" si="12"/>
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="25" spans="1:83">
       <c r="A25" s="90">
         <f t="shared" ca="1" si="10"/>
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B25" s="18" t="str">
         <f ca="1">IF(ISNUMBER(A25),INDEX(Backlog!$A:$M,$A25,B$5),"")</f>
-        <v>6.1.5</v>
+        <v>6.1.7</v>
       </c>
       <c r="C25" s="73" t="str">
         <f ca="1">IF($B25="","",INDEX(Backlog!$A:$M,$A25,C$5))</f>
@@ -45790,15 +45786,15 @@
       </c>
       <c r="E25" s="73" t="str">
         <f ca="1">IF($B25="","",INDEX(Backlog!$A:$M,$A25,E$5))</f>
-        <v>Mode intérieur</v>
+        <v>Lire un Ibeacon</v>
       </c>
       <c r="F25" s="48">
         <f ca="1">IF($B25="","",INDEX(Backlog!$A:$M,$A25,F$5))</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G25" s="66">
         <f ca="1">IF($B25="","",INDEX(Backlog!$A:$M,$A25,G$5))</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H25" s="26"/>
       <c r="I25" s="26"/>
@@ -45873,7 +45869,7 @@
       <c r="BZ25" s="84"/>
       <c r="CA25" s="21">
         <f t="shared" ca="1" si="11"/>
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="CB25" s="21">
         <f t="shared" ca="1" si="7"/>
@@ -45881,7 +45877,7 @@
       </c>
       <c r="CC25" s="21" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>Backlog!$F$78:$F$151</v>
+        <v>Backlog!$F$80:$F$151</v>
       </c>
       <c r="CD25" s="21">
         <f t="shared" ca="1" si="9"/>
@@ -45889,17 +45885,17 @@
       </c>
       <c r="CE25" s="21">
         <f t="shared" ca="1" si="12"/>
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="26" spans="1:83">
       <c r="A26" s="90">
         <f t="shared" ca="1" si="10"/>
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="B26" s="18" t="str">
         <f ca="1">IF(ISNUMBER(A26),INDEX(Backlog!$A:$M,$A26,B$5),"")</f>
-        <v>6.1.6</v>
+        <v>6.3.5</v>
       </c>
       <c r="C26" s="73" t="str">
         <f ca="1">IF($B26="","",INDEX(Backlog!$A:$M,$A26,C$5))</f>
@@ -45907,19 +45903,19 @@
       </c>
       <c r="D26" s="73" t="str">
         <f ca="1">IF($B26="","",INDEX(Backlog!$A:$M,$A26,D$5))</f>
-        <v>Capteurs</v>
+        <v>IHM</v>
       </c>
       <c r="E26" s="73" t="str">
         <f ca="1">IF($B26="","",INDEX(Backlog!$A:$M,$A26,E$5))</f>
-        <v>Mode extérieur</v>
+        <v>Navigation Avancée</v>
       </c>
       <c r="F26" s="48">
         <f ca="1">IF($B26="","",INDEX(Backlog!$A:$M,$A26,F$5))</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G26" s="66">
         <f ca="1">IF($B26="","",INDEX(Backlog!$A:$M,$A26,G$5))</f>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="H26" s="26"/>
       <c r="I26" s="26"/>
@@ -45994,7 +45990,7 @@
       <c r="BZ26" s="84"/>
       <c r="CA26" s="21">
         <f t="shared" ca="1" si="11"/>
-        <v>79</v>
+        <v>92</v>
       </c>
       <c r="CB26" s="21">
         <f t="shared" ca="1" si="7"/>
@@ -46002,45 +45998,45 @@
       </c>
       <c r="CC26" s="21" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>Backlog!$F$79:$F$151</v>
+        <v>Backlog!$F$92:$F$151</v>
       </c>
       <c r="CD26" s="21">
         <f t="shared" ca="1" si="9"/>
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="CE26" s="21">
         <f t="shared" ca="1" si="12"/>
-        <v>79</v>
+        <v>92</v>
       </c>
     </row>
     <row r="27" spans="1:83">
       <c r="A27" s="90">
         <f t="shared" ca="1" si="10"/>
-        <v>79</v>
+        <v>113</v>
       </c>
       <c r="B27" s="18" t="str">
         <f ca="1">IF(ISNUMBER(A27),INDEX(Backlog!$A:$M,$A27,B$5),"")</f>
-        <v>6.1.7</v>
+        <v>8.1.2</v>
       </c>
       <c r="C27" s="73" t="str">
         <f ca="1">IF($B27="","",INDEX(Backlog!$A:$M,$A27,C$5))</f>
-        <v>Android</v>
+        <v>Contrôle &amp; Tests</v>
       </c>
       <c r="D27" s="73" t="str">
         <f ca="1">IF($B27="","",INDEX(Backlog!$A:$M,$A27,D$5))</f>
-        <v>Capteurs</v>
+        <v>Retours sur itération précédente</v>
       </c>
       <c r="E27" s="73" t="str">
         <f ca="1">IF($B27="","",INDEX(Backlog!$A:$M,$A27,E$5))</f>
-        <v>Lire un Ibeacon</v>
+        <v>Retours sur itération 2</v>
       </c>
       <c r="F27" s="48">
         <f ca="1">IF($B27="","",INDEX(Backlog!$A:$M,$A27,F$5))</f>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="G27" s="66">
         <f ca="1">IF($B27="","",INDEX(Backlog!$A:$M,$A27,G$5))</f>
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="H27" s="26"/>
       <c r="I27" s="26"/>
@@ -46115,7 +46111,7 @@
       <c r="BZ27" s="84"/>
       <c r="CA27" s="21">
         <f t="shared" ca="1" si="11"/>
-        <v>80</v>
+        <v>114</v>
       </c>
       <c r="CB27" s="21">
         <f t="shared" ca="1" si="7"/>
@@ -46123,37 +46119,37 @@
       </c>
       <c r="CC27" s="21" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>Backlog!$F$80:$F$151</v>
+        <v>Backlog!$F$114:$F$151</v>
       </c>
       <c r="CD27" s="21">
         <f t="shared" ca="1" si="9"/>
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="CE27" s="21">
         <f t="shared" ca="1" si="12"/>
-        <v>80</v>
+        <v>114</v>
       </c>
     </row>
     <row r="28" spans="1:83">
       <c r="A28" s="90">
         <f t="shared" ca="1" si="10"/>
-        <v>91</v>
+        <v>119</v>
       </c>
       <c r="B28" s="18" t="str">
         <f ca="1">IF(ISNUMBER(A28),INDEX(Backlog!$A:$M,$A28,B$5),"")</f>
-        <v>6.3.5</v>
+        <v>8.2.3</v>
       </c>
       <c r="C28" s="73" t="str">
         <f ca="1">IF($B28="","",INDEX(Backlog!$A:$M,$A28,C$5))</f>
-        <v>Android</v>
+        <v>Contrôle &amp; Tests</v>
       </c>
       <c r="D28" s="73" t="str">
         <f ca="1">IF($B28="","",INDEX(Backlog!$A:$M,$A28,D$5))</f>
-        <v>IHM</v>
+        <v>Tests Fonctionnels</v>
       </c>
       <c r="E28" s="73" t="str">
         <f ca="1">IF($B28="","",INDEX(Backlog!$A:$M,$A28,E$5))</f>
-        <v>Navigation Avancée</v>
+        <v>Tests Fonctionnels itération 3</v>
       </c>
       <c r="F28" s="48">
         <f ca="1">IF($B28="","",INDEX(Backlog!$A:$M,$A28,F$5))</f>
@@ -46161,7 +46157,7 @@
       </c>
       <c r="G28" s="66">
         <f ca="1">IF($B28="","",INDEX(Backlog!$A:$M,$A28,G$5))</f>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="H28" s="26"/>
       <c r="I28" s="26"/>
@@ -46236,7 +46232,7 @@
       <c r="BZ28" s="84"/>
       <c r="CA28" s="21">
         <f t="shared" ca="1" si="11"/>
-        <v>92</v>
+        <v>120</v>
       </c>
       <c r="CB28" s="21">
         <f t="shared" ca="1" si="7"/>
@@ -46244,25 +46240,25 @@
       </c>
       <c r="CC28" s="21" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>Backlog!$F$92:$F$151</v>
+        <v>Backlog!$F$120:$F$151</v>
       </c>
       <c r="CD28" s="21">
         <f t="shared" ca="1" si="9"/>
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="CE28" s="21">
         <f t="shared" ca="1" si="12"/>
-        <v>92</v>
+        <v>120</v>
       </c>
     </row>
     <row r="29" spans="1:83">
       <c r="A29" s="90">
         <f t="shared" ca="1" si="10"/>
-        <v>113</v>
+        <v>124</v>
       </c>
       <c r="B29" s="18" t="str">
         <f ca="1">IF(ISNUMBER(A29),INDEX(Backlog!$A:$M,$A29,B$5),"")</f>
-        <v>8.1.2</v>
+        <v>8.3.3</v>
       </c>
       <c r="C29" s="73" t="str">
         <f ca="1">IF($B29="","",INDEX(Backlog!$A:$M,$A29,C$5))</f>
@@ -46270,19 +46266,19 @@
       </c>
       <c r="D29" s="73" t="str">
         <f ca="1">IF($B29="","",INDEX(Backlog!$A:$M,$A29,D$5))</f>
-        <v>Retours sur itération précédente</v>
+        <v>Livraison &amp; Packaging</v>
       </c>
       <c r="E29" s="73" t="str">
         <f ca="1">IF($B29="","",INDEX(Backlog!$A:$M,$A29,E$5))</f>
-        <v>Retours sur itération 2</v>
+        <v>Livraison &amp; Packaging itération 3</v>
       </c>
       <c r="F29" s="48">
         <f ca="1">IF($B29="","",INDEX(Backlog!$A:$M,$A29,F$5))</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G29" s="66">
         <f ca="1">IF($B29="","",INDEX(Backlog!$A:$M,$A29,G$5))</f>
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="H29" s="26"/>
       <c r="I29" s="26"/>
@@ -46357,7 +46353,7 @@
       <c r="BZ29" s="84"/>
       <c r="CA29" s="21">
         <f t="shared" ca="1" si="11"/>
-        <v>114</v>
+        <v>125</v>
       </c>
       <c r="CB29" s="21">
         <f t="shared" ca="1" si="7"/>
@@ -46365,45 +46361,45 @@
       </c>
       <c r="CC29" s="21" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>Backlog!$F$114:$F$151</v>
+        <v>Backlog!$F$125:$F$151</v>
       </c>
       <c r="CD29" s="21">
         <f t="shared" ca="1" si="9"/>
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="CE29" s="21">
         <f t="shared" ca="1" si="12"/>
-        <v>114</v>
+        <v>125</v>
       </c>
     </row>
     <row r="30" spans="1:83">
       <c r="A30" s="90">
         <f t="shared" ca="1" si="10"/>
-        <v>119</v>
+        <v>130</v>
       </c>
       <c r="B30" s="18" t="str">
         <f ca="1">IF(ISNUMBER(A30),INDEX(Backlog!$A:$M,$A30,B$5),"")</f>
-        <v>8.2.3</v>
+        <v>9.1.4</v>
       </c>
       <c r="C30" s="73" t="str">
         <f ca="1">IF($B30="","",INDEX(Backlog!$A:$M,$A30,C$5))</f>
-        <v>Contrôle &amp; Tests</v>
+        <v>Conception &amp; Spec</v>
       </c>
       <c r="D30" s="73" t="str">
         <f ca="1">IF($B30="","",INDEX(Backlog!$A:$M,$A30,D$5))</f>
-        <v>Tests Fonctionnels</v>
+        <v>Conception</v>
       </c>
       <c r="E30" s="73" t="str">
         <f ca="1">IF($B30="","",INDEX(Backlog!$A:$M,$A30,E$5))</f>
-        <v>Tests Fonctionnels itération 3</v>
+        <v>Conception pré-itération 4</v>
       </c>
       <c r="F30" s="48">
         <f ca="1">IF($B30="","",INDEX(Backlog!$A:$M,$A30,F$5))</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G30" s="66">
         <f ca="1">IF($B30="","",INDEX(Backlog!$A:$M,$A30,G$5))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H30" s="26"/>
       <c r="I30" s="26"/>
@@ -46478,7 +46474,7 @@
       <c r="BZ30" s="84"/>
       <c r="CA30" s="21">
         <f t="shared" ca="1" si="11"/>
-        <v>120</v>
+        <v>131</v>
       </c>
       <c r="CB30" s="21">
         <f t="shared" ca="1" si="7"/>
@@ -46486,7 +46482,7 @@
       </c>
       <c r="CC30" s="21" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>Backlog!$F$120:$F$151</v>
+        <v>Backlog!$F$131:$F$151</v>
       </c>
       <c r="CD30" s="21">
         <f t="shared" ca="1" si="9"/>
@@ -46494,37 +46490,37 @@
       </c>
       <c r="CE30" s="21">
         <f t="shared" ca="1" si="12"/>
-        <v>120</v>
+        <v>131</v>
       </c>
     </row>
     <row r="31" spans="1:83">
       <c r="A31" s="90">
         <f t="shared" ca="1" si="10"/>
-        <v>124</v>
+        <v>135</v>
       </c>
       <c r="B31" s="18" t="str">
         <f ca="1">IF(ISNUMBER(A31),INDEX(Backlog!$A:$M,$A31,B$5),"")</f>
-        <v>8.3.3</v>
+        <v>9.2.4</v>
       </c>
       <c r="C31" s="73" t="str">
         <f ca="1">IF($B31="","",INDEX(Backlog!$A:$M,$A31,C$5))</f>
-        <v>Contrôle &amp; Tests</v>
+        <v>Conception &amp; Spec</v>
       </c>
       <c r="D31" s="73" t="str">
         <f ca="1">IF($B31="","",INDEX(Backlog!$A:$M,$A31,D$5))</f>
-        <v>Livraison &amp; Packaging</v>
+        <v>Spécification</v>
       </c>
       <c r="E31" s="73" t="str">
         <f ca="1">IF($B31="","",INDEX(Backlog!$A:$M,$A31,E$5))</f>
-        <v>Livraison &amp; Packaging itération 3</v>
+        <v>Spécification pré-itération 4</v>
       </c>
       <c r="F31" s="48">
         <f ca="1">IF($B31="","",INDEX(Backlog!$A:$M,$A31,F$5))</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G31" s="66">
         <f ca="1">IF($B31="","",INDEX(Backlog!$A:$M,$A31,G$5))</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H31" s="26"/>
       <c r="I31" s="26"/>
@@ -46599,7 +46595,7 @@
       <c r="BZ31" s="84"/>
       <c r="CA31" s="21">
         <f t="shared" ca="1" si="11"/>
-        <v>125</v>
+        <v>136</v>
       </c>
       <c r="CB31" s="21">
         <f t="shared" ca="1" si="7"/>
@@ -46607,7 +46603,7 @@
       </c>
       <c r="CC31" s="21" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>Backlog!$F$125:$F$151</v>
+        <v>Backlog!$F$136:$F$151</v>
       </c>
       <c r="CD31" s="21">
         <f t="shared" ca="1" si="9"/>
@@ -46615,29 +46611,29 @@
       </c>
       <c r="CE31" s="21">
         <f t="shared" ca="1" si="12"/>
-        <v>125</v>
+        <v>136</v>
       </c>
     </row>
     <row r="32" spans="1:83">
       <c r="A32" s="90">
         <f t="shared" ca="1" si="10"/>
-        <v>130</v>
+        <v>139</v>
       </c>
       <c r="B32" s="18" t="str">
         <f ca="1">IF(ISNUMBER(A32),INDEX(Backlog!$A:$M,$A32,B$5),"")</f>
-        <v>9.1.4</v>
+        <v>10.1.3</v>
       </c>
       <c r="C32" s="73" t="str">
         <f ca="1">IF($B32="","",INDEX(Backlog!$A:$M,$A32,C$5))</f>
-        <v>Conception &amp; Spec</v>
+        <v>Gestion de projet</v>
       </c>
       <c r="D32" s="73" t="str">
         <f ca="1">IF($B32="","",INDEX(Backlog!$A:$M,$A32,D$5))</f>
-        <v>Conception</v>
+        <v>Réunions</v>
       </c>
       <c r="E32" s="73" t="str">
         <f ca="1">IF($B32="","",INDEX(Backlog!$A:$M,$A32,E$5))</f>
-        <v>Conception pré-itération 4</v>
+        <v>Réunions itération 3</v>
       </c>
       <c r="F32" s="48">
         <f ca="1">IF($B32="","",INDEX(Backlog!$A:$M,$A32,F$5))</f>
@@ -46645,7 +46641,7 @@
       </c>
       <c r="G32" s="66">
         <f ca="1">IF($B32="","",INDEX(Backlog!$A:$M,$A32,G$5))</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H32" s="26"/>
       <c r="I32" s="26"/>
@@ -46720,7 +46716,7 @@
       <c r="BZ32" s="84"/>
       <c r="CA32" s="21">
         <f t="shared" ca="1" si="11"/>
-        <v>131</v>
+        <v>140</v>
       </c>
       <c r="CB32" s="21">
         <f t="shared" ca="1" si="7"/>
@@ -46728,37 +46724,37 @@
       </c>
       <c r="CC32" s="21" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>Backlog!$F$131:$F$151</v>
+        <v>Backlog!$F$140:$F$151</v>
       </c>
       <c r="CD32" s="21">
         <f t="shared" ca="1" si="9"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="CE32" s="21">
         <f t="shared" ca="1" si="12"/>
-        <v>131</v>
+        <v>140</v>
       </c>
     </row>
     <row r="33" spans="1:83">
       <c r="A33" s="90">
         <f t="shared" ca="1" si="10"/>
-        <v>135</v>
+        <v>144</v>
       </c>
       <c r="B33" s="18" t="str">
         <f ca="1">IF(ISNUMBER(A33),INDEX(Backlog!$A:$M,$A33,B$5),"")</f>
-        <v>9.2.4</v>
+        <v>10.2.3</v>
       </c>
       <c r="C33" s="73" t="str">
         <f ca="1">IF($B33="","",INDEX(Backlog!$A:$M,$A33,C$5))</f>
-        <v>Conception &amp; Spec</v>
+        <v>Gestion de projet</v>
       </c>
       <c r="D33" s="73" t="str">
         <f ca="1">IF($B33="","",INDEX(Backlog!$A:$M,$A33,D$5))</f>
-        <v>Spécification</v>
+        <v>Backlog</v>
       </c>
       <c r="E33" s="73" t="str">
         <f ca="1">IF($B33="","",INDEX(Backlog!$A:$M,$A33,E$5))</f>
-        <v>Spécification pré-itération 4</v>
+        <v>Mise à jour Backlog itération 3</v>
       </c>
       <c r="F33" s="48">
         <f ca="1">IF($B33="","",INDEX(Backlog!$A:$M,$A33,F$5))</f>
@@ -46766,7 +46762,7 @@
       </c>
       <c r="G33" s="66">
         <f ca="1">IF($B33="","",INDEX(Backlog!$A:$M,$A33,G$5))</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H33" s="26"/>
       <c r="I33" s="26"/>
@@ -46841,7 +46837,7 @@
       <c r="BZ33" s="84"/>
       <c r="CA33" s="21">
         <f t="shared" ca="1" si="11"/>
-        <v>136</v>
+        <v>145</v>
       </c>
       <c r="CB33" s="21">
         <f t="shared" ca="1" si="7"/>
@@ -46849,7 +46845,7 @@
       </c>
       <c r="CC33" s="21" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>Backlog!$F$136:$F$151</v>
+        <v>Backlog!$F$145:$F$151</v>
       </c>
       <c r="CD33" s="21">
         <f t="shared" ca="1" si="9"/>
@@ -46857,29 +46853,29 @@
       </c>
       <c r="CE33" s="21">
         <f t="shared" ca="1" si="12"/>
-        <v>136</v>
+        <v>145</v>
       </c>
     </row>
     <row r="34" spans="1:83">
       <c r="A34" s="90">
         <f t="shared" ca="1" si="10"/>
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="B34" s="18" t="str">
         <f ca="1">IF(ISNUMBER(A34),INDEX(Backlog!$A:$M,$A34,B$5),"")</f>
-        <v>10.1.3</v>
+        <v>11.1.3</v>
       </c>
       <c r="C34" s="73" t="str">
         <f ca="1">IF($B34="","",INDEX(Backlog!$A:$M,$A34,C$5))</f>
-        <v>Gestion de projet</v>
+        <v>Documentation</v>
       </c>
       <c r="D34" s="73" t="str">
         <f ca="1">IF($B34="","",INDEX(Backlog!$A:$M,$A34,D$5))</f>
-        <v>Réunions</v>
+        <v>Documentation</v>
       </c>
       <c r="E34" s="73" t="str">
         <f ca="1">IF($B34="","",INDEX(Backlog!$A:$M,$A34,E$5))</f>
-        <v>Réunions itération 3</v>
+        <v>Documentation itération 3</v>
       </c>
       <c r="F34" s="48">
         <f ca="1">IF($B34="","",INDEX(Backlog!$A:$M,$A34,F$5))</f>
@@ -46887,7 +46883,7 @@
       </c>
       <c r="G34" s="66">
         <f ca="1">IF($B34="","",INDEX(Backlog!$A:$M,$A34,G$5))</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H34" s="26"/>
       <c r="I34" s="26"/>
@@ -46962,7 +46958,7 @@
       <c r="BZ34" s="84"/>
       <c r="CA34" s="21">
         <f t="shared" ca="1" si="11"/>
-        <v>140</v>
+        <v>150</v>
       </c>
       <c r="CB34" s="21">
         <f t="shared" ca="1" si="7"/>
@@ -46970,45 +46966,45 @@
       </c>
       <c r="CC34" s="21" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>Backlog!$F$140:$F$151</v>
+        <v>Backlog!$F$150:$F$151</v>
       </c>
       <c r="CD34" s="21">
         <f t="shared" ca="1" si="9"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="CE34" s="21">
         <f t="shared" ca="1" si="12"/>
-        <v>140</v>
+        <v>150</v>
       </c>
     </row>
     <row r="35" spans="1:83">
-      <c r="A35" s="90">
+      <c r="A35" s="90" t="e">
         <f t="shared" ca="1" si="10"/>
-        <v>144</v>
+        <v>#VALUE!</v>
       </c>
       <c r="B35" s="18" t="str">
         <f ca="1">IF(ISNUMBER(A35),INDEX(Backlog!$A:$M,$A35,B$5),"")</f>
-        <v>10.2.3</v>
+        <v/>
       </c>
       <c r="C35" s="73" t="str">
         <f ca="1">IF($B35="","",INDEX(Backlog!$A:$M,$A35,C$5))</f>
-        <v>Gestion de projet</v>
+        <v/>
       </c>
       <c r="D35" s="73" t="str">
         <f ca="1">IF($B35="","",INDEX(Backlog!$A:$M,$A35,D$5))</f>
-        <v>Backlog</v>
+        <v/>
       </c>
       <c r="E35" s="73" t="str">
         <f ca="1">IF($B35="","",INDEX(Backlog!$A:$M,$A35,E$5))</f>
-        <v>Mise à jour Backlog itération 3</v>
-      </c>
-      <c r="F35" s="48">
+        <v/>
+      </c>
+      <c r="F35" s="48" t="str">
         <f ca="1">IF($B35="","",INDEX(Backlog!$A:$M,$A35,F$5))</f>
-        <v>1</v>
-      </c>
-      <c r="G35" s="66">
+        <v/>
+      </c>
+      <c r="G35" s="66" t="str">
         <f ca="1">IF($B35="","",INDEX(Backlog!$A:$M,$A35,G$5))</f>
-        <v>2</v>
+        <v/>
       </c>
       <c r="H35" s="26"/>
       <c r="I35" s="26"/>
@@ -47081,55 +47077,55 @@
       <c r="BX35" s="26"/>
       <c r="BY35" s="26"/>
       <c r="BZ35" s="84"/>
-      <c r="CA35" s="21">
+      <c r="CA35" s="21" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>145</v>
-      </c>
-      <c r="CB35" s="21">
+        <v/>
+      </c>
+      <c r="CB35" s="21" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>151</v>
-      </c>
-      <c r="CC35" s="21" t="str">
+        <v/>
+      </c>
+      <c r="CC35" s="21" t="e">
         <f t="shared" ca="1" si="8"/>
-        <v>Backlog!$F$145:$F$151</v>
-      </c>
-      <c r="CD35" s="21">
+        <v>#VALUE!</v>
+      </c>
+      <c r="CD35" s="21" t="e">
         <f t="shared" ca="1" si="9"/>
-        <v>5</v>
-      </c>
-      <c r="CE35" s="21">
+        <v>#N/A</v>
+      </c>
+      <c r="CE35" s="21" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>145</v>
+        <v/>
       </c>
     </row>
     <row r="36" spans="1:83">
-      <c r="A36" s="90">
+      <c r="A36" s="90" t="e">
         <f t="shared" ca="1" si="10"/>
-        <v>149</v>
+        <v>#VALUE!</v>
       </c>
       <c r="B36" s="18" t="str">
         <f ca="1">IF(ISNUMBER(A36),INDEX(Backlog!$A:$M,$A36,B$5),"")</f>
-        <v>11.1.3</v>
+        <v/>
       </c>
       <c r="C36" s="73" t="str">
         <f ca="1">IF($B36="","",INDEX(Backlog!$A:$M,$A36,C$5))</f>
-        <v>Documentation</v>
+        <v/>
       </c>
       <c r="D36" s="73" t="str">
         <f ca="1">IF($B36="","",INDEX(Backlog!$A:$M,$A36,D$5))</f>
-        <v>Documentation</v>
+        <v/>
       </c>
       <c r="E36" s="73" t="str">
         <f ca="1">IF($B36="","",INDEX(Backlog!$A:$M,$A36,E$5))</f>
-        <v>Documentation itération 3</v>
-      </c>
-      <c r="F36" s="48">
+        <v/>
+      </c>
+      <c r="F36" s="48" t="str">
         <f ca="1">IF($B36="","",INDEX(Backlog!$A:$M,$A36,F$5))</f>
-        <v>1</v>
-      </c>
-      <c r="G36" s="66">
+        <v/>
+      </c>
+      <c r="G36" s="66" t="str">
         <f ca="1">IF($B36="","",INDEX(Backlog!$A:$M,$A36,G$5))</f>
-        <v>4</v>
+        <v/>
       </c>
       <c r="H36" s="26"/>
       <c r="I36" s="26"/>
@@ -47202,25 +47198,25 @@
       <c r="BX36" s="26"/>
       <c r="BY36" s="26"/>
       <c r="BZ36" s="84"/>
-      <c r="CA36" s="21">
+      <c r="CA36" s="21" t="e">
         <f t="shared" ca="1" si="11"/>
-        <v>150</v>
-      </c>
-      <c r="CB36" s="21">
+        <v>#VALUE!</v>
+      </c>
+      <c r="CB36" s="21" t="e">
         <f t="shared" ca="1" si="7"/>
-        <v>151</v>
-      </c>
-      <c r="CC36" s="21" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="CC36" s="21" t="e">
         <f t="shared" ca="1" si="8"/>
-        <v>Backlog!$F$150:$F$151</v>
-      </c>
-      <c r="CD36" s="21">
+        <v>#VALUE!</v>
+      </c>
+      <c r="CD36" s="21" t="e">
         <f t="shared" ca="1" si="9"/>
-        <v>5</v>
-      </c>
-      <c r="CE36" s="21">
+        <v>#VALUE!</v>
+      </c>
+      <c r="CE36" s="21" t="e">
         <f t="shared" ca="1" si="12"/>
-        <v>150</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="37" spans="1:83">
@@ -47323,13 +47319,13 @@
       <c r="BX37" s="26"/>
       <c r="BY37" s="26"/>
       <c r="BZ37" s="84"/>
-      <c r="CA37" s="21" t="str">
+      <c r="CA37" s="21" t="e">
         <f t="shared" ca="1" si="11"/>
-        <v/>
-      </c>
-      <c r="CB37" s="21" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="CB37" s="21" t="e">
         <f t="shared" ca="1" si="7"/>
-        <v/>
+        <v>#VALUE!</v>
       </c>
       <c r="CC37" s="21" t="e">
         <f t="shared" ca="1" si="8"/>
@@ -47337,11 +47333,11 @@
       </c>
       <c r="CD37" s="21" t="e">
         <f t="shared" ca="1" si="9"/>
-        <v>#N/A</v>
-      </c>
-      <c r="CE37" s="21" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="CE37" s="21" t="e">
         <f t="shared" ca="1" si="12"/>
-        <v/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="38" spans="1:83">

</xml_diff>